<commit_message>
Changes made in xl sheet
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:O20"/>
 </workbook>
 </file>
 
@@ -519,7 +518,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -568,7 +567,7 @@
         <v>26</v>
       </c>
       <c r="C4">
-        <v>25000</v>
+        <v>30000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>